<commit_message>
Pressget: These are the changes I made
Check every details of my changes if its not correct syntactically , please correct it sir
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cleargo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Cleargo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73514680-02EF-4695-8A83-D3125B75EC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="5520"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -69,12 +70,18 @@
   </si>
   <si>
     <t>josh@gmail.com</t>
+  </si>
+  <si>
+    <t>ICT</t>
+  </si>
+  <si>
+    <t>Basic and Applied Sciences</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,11 +403,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,17 +474,17 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>